<commit_message>
unpdate marine fungi and protists
</commit_message>
<xml_diff>
--- a/fungi/marine_fungi/marine_fungi_data.xlsx
+++ b/fungi/marine_fungi/marine_fungi_data.xlsx
@@ -1300,7 +1300,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1333,10 +1333,10 @@
         <v>34</v>
       </c>
       <c r="B3" s="1" t="n">
-        <v>0.23</v>
+        <v>0.35</v>
       </c>
       <c r="C3" s="1" t="n">
-        <v>0.95</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1344,10 +1344,10 @@
         <v>35</v>
       </c>
       <c r="B4" s="1" t="n">
-        <v>0.29</v>
+        <v>0.44</v>
       </c>
       <c r="C4" s="1" t="n">
-        <v>1.29</v>
+        <v>1.98</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -1355,10 +1355,10 @@
         <v>36</v>
       </c>
       <c r="B5" s="1" t="n">
-        <v>0.37</v>
+        <v>0.53</v>
       </c>
       <c r="C5" s="1" t="n">
-        <v>0.37</v>
+        <v>0.53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>